<commit_message>
Alteração no Product Backlog com relação as Sprints
</commit_message>
<xml_diff>
--- a/trunk/doc/PAN-2014-1-Modelo-Product-Backlog.xlsx
+++ b/trunk/doc/PAN-2014-1-Modelo-Product-Backlog.xlsx
@@ -978,7 +978,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -1070,7 +1070,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="15"/>
@@ -1097,7 +1097,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>22</v>
@@ -1132,7 +1132,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="15"/>
@@ -1164,7 +1164,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="15"/>
@@ -1193,7 +1193,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>11</v>
@@ -1227,7 +1227,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="15"/>
@@ -1463,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="15"/>
@@ -1637,7 +1637,7 @@
         <v>13</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="15"/>

</xml_diff>